<commit_message>
more BoM edits done & submitted for quote
</commit_message>
<xml_diff>
--- a/allegro/GerberMJL/BoM-edited for PCB Train.xlsx
+++ b/allegro/GerberMJL/BoM-edited for PCB Train.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dune_GIB\upenn-dune-gib\allegro\GerberMJL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5009E2A-EAE5-400D-894D-8ED37576EC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B498B774-FA88-4412-9DDF-0B4799A20905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{66CE21EB-B273-4EBF-A88B-400297C7A1D2}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{66CE21EB-B273-4EBF-A88B-400297C7A1D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="338">
   <si>
     <t>Item Number</t>
   </si>
@@ -1023,9 +1023,6 @@
     <t>RMCF0603FT143K</t>
   </si>
   <si>
-    <t>obsolete?</t>
-  </si>
-  <si>
     <t>MAX9371ESA+</t>
   </si>
   <si>
@@ -1051,6 +1048,12 @@
   </si>
   <si>
     <t>Obsolete - alternative P/N</t>
+  </si>
+  <si>
+    <t>obsolete? Seems various chip-brokers have stock though.</t>
+  </si>
+  <si>
+    <t>Hard to get hold of!</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1137,7 +1140,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -1476,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E95D90-0A23-4E73-9F6F-B31BFA4E651F}">
   <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="C72" workbookViewId="0">
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2691,11 +2693,11 @@
       <c r="D28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>94</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>95</v>
@@ -2719,7 +2721,7 @@
         <v>13</v>
       </c>
       <c r="O28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -3189,9 +3191,7 @@
       <c r="E40" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>185</v>
-      </c>
+      <c r="F40" s="2"/>
       <c r="G40" s="2" t="s">
         <v>123</v>
       </c>
@@ -3230,9 +3230,7 @@
       <c r="E41" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>185</v>
-      </c>
+      <c r="F41" s="2"/>
       <c r="G41" s="2" t="s">
         <v>125</v>
       </c>
@@ -4107,9 +4105,7 @@
       <c r="E61" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>299</v>
-      </c>
+      <c r="F61" s="2"/>
       <c r="G61" s="2" t="s">
         <v>187</v>
       </c>
@@ -4550,9 +4546,7 @@
       <c r="E71" t="s">
         <v>324</v>
       </c>
-      <c r="F71" s="2" t="s">
-        <v>185</v>
-      </c>
+      <c r="F71" s="2"/>
       <c r="G71" s="2" t="s">
         <v>214</v>
       </c>
@@ -4683,7 +4677,7 @@
         <v>226</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>227</v>
@@ -4726,9 +4720,7 @@
       <c r="E75" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>185</v>
-      </c>
+      <c r="F75" s="2"/>
       <c r="G75" s="4" t="s">
         <v>230</v>
       </c>
@@ -4764,7 +4756,7 @@
       <c r="D76" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E76" s="11" t="s">
+      <c r="E76" s="10" t="s">
         <v>231</v>
       </c>
       <c r="F76" s="2" t="s">
@@ -4791,8 +4783,8 @@
       <c r="M76" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O76" s="12" t="s">
-        <v>327</v>
+      <c r="O76" s="11" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
@@ -4809,10 +4801,10 @@
         <v>13</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>234</v>
@@ -4824,10 +4816,10 @@
         <v>13</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>13</v>
@@ -4836,7 +4828,7 @@
         <v>13</v>
       </c>
       <c r="O77" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
@@ -4853,10 +4845,10 @@
         <v>13</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>235</v>
@@ -4868,10 +4860,10 @@
         <v>13</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>13</v>
@@ -4879,8 +4871,8 @@
       <c r="M78" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O78" s="10" t="s">
-        <v>329</v>
+      <c r="O78" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
@@ -4965,7 +4957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -5006,7 +4998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -5023,7 +5015,7 @@
         <v>243</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>244</v>
@@ -5047,7 +5039,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -5088,7 +5080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -5104,9 +5096,7 @@
       <c r="E84" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F84" s="2" t="s">
-        <v>185</v>
-      </c>
+      <c r="F84" s="2"/>
       <c r="G84" s="2" t="s">
         <v>248</v>
       </c>
@@ -5129,7 +5119,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -5170,7 +5160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -5211,7 +5201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -5252,7 +5242,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -5293,7 +5283,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -5334,7 +5324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -5375,7 +5365,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -5416,7 +5406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -5457,7 +5447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -5498,7 +5488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -5539,7 +5529,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -5580,7 +5570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -5593,7 +5583,7 @@
       <c r="D96" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="E96" s="10" t="s">
         <v>271</v>
       </c>
       <c r="F96" s="2" t="s">
@@ -5619,6 +5609,9 @@
       </c>
       <c r="M96" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="O96" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.3">
@@ -5676,10 +5669,10 @@
         <v>13</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>276</v>

</xml_diff>